<commit_message>
update excel file and create pcb
</commit_message>
<xml_diff>
--- a/comandos monitor de agua.xlsx
+++ b/comandos monitor de agua.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wonka\OneDrive\Escritorio\git monitor agua\monitor-consumo-agua\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB897CEE-2258-48F3-B99A-ABB2DDA9B1C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A41FBF-BCA8-451A-BE98-74B192459F70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{8BFFBC1D-2DF0-4176-A9C5-D8A9D9DB23E7}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t xml:space="preserve">Comando </t>
-  </si>
-  <si>
-    <t>Tipo de consulta</t>
   </si>
   <si>
     <t>Accion</t>
@@ -314,12 +311,6 @@
     <t>{ tank_id: 1, liters:  4500 , last_filled: date , max_capacity }</t>
   </si>
   <si>
-    <t>hecho</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>consumo mes anterior</t>
   </si>
   <si>
@@ -329,9 +320,6 @@
     <t>devuelve el consumo del mes hasta el momento de ambos monitores</t>
   </si>
   <si>
-    <t>x x</t>
-  </si>
-  <si>
     <t xml:space="preserve">{"device": "ingreso",  "liters": 4.5}   =&gt; {device: "nombre del dispositivo",  liters: 4.5,  date: "2023-11-22T12:34:56Z" } servidor agrega la hora de ingreso </t>
   </si>
   <si>
@@ -345,6 +333,18 @@
   </si>
   <si>
     <t>water_tank/capacity</t>
+  </si>
+  <si>
+    <t>Tipo de operacion</t>
+  </si>
+  <si>
+    <t>{nube: 15.5}</t>
+  </si>
+  <si>
+    <t>water_tank/full</t>
+  </si>
+  <si>
+    <t>{capacity: x}</t>
   </si>
 </sst>
 </file>
@@ -712,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6FB90F-6080-4A20-BFF1-124E28EED8E9}">
-  <dimension ref="D5:G46"/>
+  <dimension ref="E5:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -725,321 +725,304 @@
     <col min="7" max="7" width="138.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:7">
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
+    <row r="5" spans="5:7">
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="6" spans="5:7">
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7">
+      <c r="E7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="4:7">
-      <c r="D6" t="s">
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="5:7">
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="4:7">
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="10" spans="5:7">
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7">
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7">
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="5:7">
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="4:7">
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="4:7">
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="5:7">
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="4:7">
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" t="s">
+    <row r="13" spans="5:7">
+      <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="4:7">
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" t="s">
+    <row r="14" spans="5:7">
+      <c r="E14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="4:7">
-      <c r="D14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
         <v>16</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="5:7">
       <c r="G20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="5:7">
       <c r="E21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="5:7">
       <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
         <v>19</v>
-      </c>
-      <c r="F22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="23" spans="5:7">
       <c r="E23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="5:7">
       <c r="F24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="5:7">
       <c r="E25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="5:7">
       <c r="F26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="5:7">
       <c r="E28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="5:7">
       <c r="F29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="5:7">
       <c r="E30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="5:7">
       <c r="F31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="5:7">
       <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" t="s">
         <v>32</v>
-      </c>
-      <c r="F33" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="34" spans="5:7">
       <c r="F34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="5:7">
       <c r="E36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="5:7">
       <c r="F37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="5:7">
+      <c r="E39" t="s">
+        <v>53</v>
+      </c>
       <c r="G39" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="5:7">
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>36</v>
-      </c>
-      <c r="F40" t="s">
-        <v>53</v>
-      </c>
-      <c r="G40" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="41" spans="5:7">
       <c r="E41" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F41" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7">
+      <c r="E42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" t="s">
+        <v>50</v>
+      </c>
+      <c r="G42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" ht="15.75">
+      <c r="E46" t="s">
+        <v>39</v>
+      </c>
+      <c r="F46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7">
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7">
+      <c r="G49" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="5:7" ht="15.75">
-      <c r="E45" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" t="s">
-        <v>41</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="5:7">
-      <c r="E46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>